<commit_message>
Updates related to Race-Ethnicity Readme
</commit_message>
<xml_diff>
--- a/Methodology/SWANA_SoAsian_Ancestry.xlsx
+++ b/Methodology/SWANA_SoAsian_Ancestry.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B38"/>
+  <dimension ref="A1:B49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -396,7 +396,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Arab</t>
+          <t>Amazigh</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -408,7 +408,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Arabic</t>
+          <t>Arab</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -420,7 +420,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Armenian</t>
+          <t>Arabic</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -432,7 +432,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Assyrian</t>
+          <t>Armenian</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -444,7 +444,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Bahraini</t>
+          <t>Assyrian</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -456,7 +456,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Berber</t>
+          <t>Azerbaijan</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -468,7 +468,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Chaldean</t>
+          <t>Bahraini</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -480,7 +480,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Egyptian</t>
+          <t>Berber</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -492,187 +492,264 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Emirati</t>
+          <t>Chaldean</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Iranian</t>
+          <t>Copt</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Iraqi</t>
+          <t>Djiboutian</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Israeli</t>
+          <t>Egyptian</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Jordanian</t>
+          <t>Emirati</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Kurdish</t>
+          <t>Iranian</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Kuwaiti</t>
+          <t>Iraqi</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Lebanese</t>
+          <t>Israeli</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Libyan</t>
+          <t>Jordanian</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Mid East</t>
+          <t>Kurdish</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Mideast</t>
+          <t>Kuwaiti</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Middle Eastern</t>
+          <t>Lebanese</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Moroccan</t>
+          <t>Levantine</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>North African</t>
+          <t>Libyan</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Omani</t>
+          <t>Mauritanian</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Other Arab</t>
+          <t>Mid East</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Palestinian</t>
+          <t>Mideast</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Qatari</t>
+          <t>Middle Eastern</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Saudi</t>
+          <t>Middle Eastern or North African Responses, not elsewhere classified</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Saudi Arabian</t>
+          <t>Moroccan</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Sudanese</t>
+          <t>North African</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Syriac</t>
+          <t>Omani</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Syrian</t>
+          <t>Other Arab</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Tunisian</t>
+          <t>Palestinian</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Turkish</t>
+          <t>Qatari</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Yazidi</t>
+          <t>Saudi</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
+        <is>
+          <t>Saudi Arabian</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Somali</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Southwest Asian or North African</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Sudanese</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>SWANA</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Syriac</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>Syrian</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>Tunisian</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>Turkish</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>West Asian</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>Yazidi</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
         <is>
           <t>Yemeni</t>
         </is>

</xml_diff>